<commit_message>
Added Data Standardisation and Cleaned Data
</commit_message>
<xml_diff>
--- a/FilePipeline/A_InputData/PopulusInputData.xlsx
+++ b/FilePipeline/A_InputData/PopulusInputData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365abdn-my.sharepoint.com/personal/u03be21_abdn_ac_uk/Documents/Documents/CS4042 DE 2/Assessment-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Assessment-2\BrokenData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5217A0AD-54C3-4F6E-803F-AAB25C275870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F7217-87DD-43D9-8D59-CF9100531998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="666" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="666" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="35" r:id="rId1"/>
@@ -3569,7 +3569,7 @@
   </sheetPr>
   <dimension ref="A1:IV87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -4186,8 +4186,8 @@
   <dimension ref="A1:BI267"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="12" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S58" sqref="S58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" zeroHeight="1"/>
@@ -4692,9 +4692,7 @@
       <c r="F17" s="147">
         <v>1824</v>
       </c>
-      <c r="G17" s="147">
-        <v>2689</v>
-      </c>
+      <c r="G17" s="147"/>
       <c r="H17" s="147">
         <v>3941</v>
       </c>
@@ -4710,9 +4708,7 @@
       <c r="L17" s="147">
         <v>15919</v>
       </c>
-      <c r="M17" s="147">
-        <v>25691</v>
-      </c>
+      <c r="M17" s="147"/>
       <c r="N17" s="147">
         <v>39232</v>
       </c>
@@ -4728,9 +4724,7 @@
       <c r="R17" s="147">
         <v>36606</v>
       </c>
-      <c r="S17" s="147">
-        <v>30026</v>
-      </c>
+      <c r="S17" s="147"/>
       <c r="T17" s="147">
         <v>349930</v>
       </c>
@@ -5002,9 +4996,7 @@
       <c r="F22" s="147">
         <v>1230</v>
       </c>
-      <c r="G22" s="147">
-        <v>1529</v>
-      </c>
+      <c r="G22" s="147"/>
       <c r="H22" s="147">
         <v>1958</v>
       </c>
@@ -5079,9 +5071,7 @@
       <c r="K23" s="147">
         <v>73018</v>
       </c>
-      <c r="L23" s="147">
-        <v>71921</v>
-      </c>
+      <c r="L23" s="147"/>
       <c r="M23" s="147">
         <v>66974</v>
       </c>
@@ -5215,9 +5205,7 @@
       <c r="O25" s="147">
         <v>73435</v>
       </c>
-      <c r="P25" s="147">
-        <v>64812</v>
-      </c>
+      <c r="P25" s="147"/>
       <c r="Q25" s="147">
         <v>45098</v>
       </c>
@@ -5387,9 +5375,7 @@
       <c r="C29" s="149">
         <v>814704</v>
       </c>
-      <c r="D29" s="149">
-        <v>816592</v>
-      </c>
+      <c r="D29" s="149"/>
       <c r="E29" s="149">
         <v>749330</v>
       </c>
@@ -5758,9 +5744,7 @@
       <c r="H36" s="147">
         <v>157</v>
       </c>
-      <c r="I36" s="147">
-        <v>171</v>
-      </c>
+      <c r="I36" s="147"/>
       <c r="J36" s="147">
         <v>245</v>
       </c>
@@ -5779,9 +5763,7 @@
       <c r="O36" s="147">
         <v>4010</v>
       </c>
-      <c r="P36" s="147">
-        <v>8592</v>
-      </c>
+      <c r="P36" s="147"/>
       <c r="Q36" s="147">
         <v>14670</v>
       </c>
@@ -5808,9 +5790,7 @@
       <c r="D37" s="147">
         <v>2304</v>
       </c>
-      <c r="E37" s="147">
-        <v>3367</v>
-      </c>
+      <c r="E37" s="147"/>
       <c r="F37" s="147">
         <v>4767</v>
       </c>
@@ -6077,12 +6057,8 @@
       <c r="K41" s="147">
         <v>107334</v>
       </c>
-      <c r="L41" s="147">
-        <v>106524</v>
-      </c>
-      <c r="M41" s="147">
-        <v>96615</v>
-      </c>
+      <c r="L41" s="147"/>
+      <c r="M41" s="147"/>
       <c r="N41" s="147">
         <v>88123</v>
       </c>
@@ -6127,9 +6103,7 @@
       <c r="G42" s="147">
         <v>688</v>
       </c>
-      <c r="H42" s="147">
-        <v>1030</v>
-      </c>
+      <c r="H42" s="147"/>
       <c r="I42" s="147">
         <v>1626</v>
       </c>
@@ -6394,9 +6368,7 @@
       <c r="F47" s="149">
         <v>772711</v>
       </c>
-      <c r="G47" s="149">
-        <v>884837</v>
-      </c>
+      <c r="G47" s="149"/>
       <c r="H47" s="149">
         <v>948691</v>
       </c>
@@ -6427,9 +6399,7 @@
       <c r="Q47" s="149">
         <v>429281</v>
       </c>
-      <c r="R47" s="149">
-        <v>302129</v>
-      </c>
+      <c r="R47" s="149"/>
       <c r="S47" s="149">
         <v>331903</v>
       </c>
@@ -6718,9 +6688,7 @@
       <c r="P53" s="147">
         <v>118787</v>
       </c>
-      <c r="Q53" s="147">
-        <v>97289</v>
-      </c>
+      <c r="Q53" s="147"/>
       <c r="R53" s="147">
         <v>67559</v>
       </c>
@@ -6738,9 +6706,7 @@
       <c r="B54" s="147">
         <v>92</v>
       </c>
-      <c r="C54" s="147">
-        <v>107</v>
-      </c>
+      <c r="C54" s="147"/>
       <c r="D54" s="147">
         <v>105</v>
       </c>
@@ -6762,9 +6728,7 @@
       <c r="J54" s="147">
         <v>539</v>
       </c>
-      <c r="K54" s="147">
-        <v>915</v>
-      </c>
+      <c r="K54" s="147"/>
       <c r="L54" s="147">
         <v>1566</v>
       </c>
@@ -6812,9 +6776,7 @@
       <c r="F55" s="147">
         <v>9472</v>
       </c>
-      <c r="G55" s="147">
-        <v>13648</v>
-      </c>
+      <c r="G55" s="147"/>
       <c r="H55" s="147">
         <v>21067</v>
       </c>
@@ -7022,9 +6984,7 @@
       <c r="N58" s="147">
         <v>52123</v>
       </c>
-      <c r="O58" s="147">
-        <v>62529</v>
-      </c>
+      <c r="O58" s="147"/>
       <c r="P58" s="147">
         <v>72763</v>
       </c>
@@ -7034,9 +6994,7 @@
       <c r="R58" s="147">
         <v>45731</v>
       </c>
-      <c r="S58" s="147">
-        <v>41952</v>
-      </c>
+      <c r="S58" s="147"/>
       <c r="T58" s="147">
         <v>441109</v>
       </c>
@@ -7128,9 +7086,7 @@
       <c r="H60" s="147">
         <v>1914</v>
       </c>
-      <c r="I60" s="147">
-        <v>3020</v>
-      </c>
+      <c r="I60" s="147"/>
       <c r="J60" s="147">
         <v>4358</v>
       </c>
@@ -7426,9 +7382,7 @@
       <c r="D65" s="149">
         <v>1588051</v>
       </c>
-      <c r="E65" s="149">
-        <v>1457812</v>
-      </c>
+      <c r="E65" s="149"/>
       <c r="F65" s="149">
         <v>1579539</v>
       </c>
@@ -7963,8 +7917,8 @@
   <dimension ref="A1:AO250"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="12" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" zeroHeight="1"/>
@@ -8582,9 +8536,7 @@
       <c r="A20" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="147">
-        <v>92</v>
-      </c>
+      <c r="B20" s="147"/>
       <c r="C20" s="147">
         <v>207</v>
       </c>
@@ -8789,9 +8741,7 @@
       <c r="A24" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="151">
-        <v>752557</v>
-      </c>
+      <c r="B24" s="151"/>
       <c r="C24" s="151">
         <v>814704</v>
       </c>
@@ -8828,9 +8778,7 @@
       <c r="N24" s="151">
         <v>711159</v>
       </c>
-      <c r="O24" s="151">
-        <v>625898</v>
-      </c>
+      <c r="O24" s="151"/>
       <c r="P24" s="151">
         <v>561275</v>
       </c>
@@ -9134,9 +9082,7 @@
       <c r="I32" s="147">
         <v>38419</v>
       </c>
-      <c r="J32" s="147">
-        <v>39593</v>
-      </c>
+      <c r="J32" s="147"/>
       <c r="K32" s="147">
         <v>48039</v>
       </c>
@@ -9807,9 +9753,7 @@
       <c r="P46" s="147">
         <v>115201</v>
       </c>
-      <c r="Q46" s="147">
-        <v>105812</v>
-      </c>
+      <c r="Q46" s="147"/>
       <c r="R46" s="147">
         <v>86967</v>
       </c>
@@ -11152,7 +11096,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" zeroHeight="1"/>
@@ -11398,9 +11342,7 @@
       <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="147">
-        <v>625835</v>
-      </c>
+      <c r="B14" s="147"/>
       <c r="C14" s="147">
         <v>543047</v>
       </c>
@@ -11485,9 +11427,7 @@
       <c r="H16" s="147">
         <v>835</v>
       </c>
-      <c r="I16" s="147">
-        <v>2634</v>
-      </c>
+      <c r="I16" s="147"/>
       <c r="J16" s="147">
         <v>189162</v>
       </c>
@@ -11635,9 +11575,7 @@
       <c r="C21" s="147">
         <v>571150</v>
       </c>
-      <c r="D21" s="147">
-        <v>496662</v>
-      </c>
+      <c r="D21" s="147"/>
       <c r="E21" s="147">
         <v>175203</v>
       </c>
@@ -11821,9 +11759,7 @@
       <c r="F27" s="149">
         <v>2660026</v>
       </c>
-      <c r="G27" s="149">
-        <v>557571</v>
-      </c>
+      <c r="G27" s="149"/>
       <c r="H27" s="149">
         <v>232605</v>
       </c>
@@ -11961,7 +11897,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" zeroHeight="1"/>
@@ -12310,9 +12246,7 @@
       <c r="H15" s="147">
         <v>13548</v>
       </c>
-      <c r="I15" s="147">
-        <v>8366</v>
-      </c>
+      <c r="I15" s="147"/>
       <c r="J15" s="147">
         <v>8687</v>
       </c>
@@ -12374,9 +12308,7 @@
       <c r="B17" s="147">
         <v>705538</v>
       </c>
-      <c r="C17" s="147">
-        <v>44276</v>
-      </c>
+      <c r="C17" s="147"/>
       <c r="D17" s="147">
         <v>106421</v>
       </c>
@@ -12439,9 +12371,7 @@
       <c r="J18" s="147">
         <v>9070</v>
       </c>
-      <c r="K18" s="147">
-        <v>11163</v>
-      </c>
+      <c r="K18" s="147"/>
       <c r="L18" s="147">
         <v>18870</v>
       </c>
@@ -12609,9 +12539,7 @@
       <c r="L22" s="147">
         <v>5487</v>
       </c>
-      <c r="M22" s="147">
-        <v>234609</v>
-      </c>
+      <c r="M22" s="147"/>
     </row>
     <row r="23" spans="1:44" ht="11.1" customHeight="1">
       <c r="A23" s="18" t="s">
@@ -12626,9 +12554,7 @@
       <c r="D23" s="147">
         <v>152721</v>
       </c>
-      <c r="E23" s="147">
-        <v>76853</v>
-      </c>
+      <c r="E23" s="147"/>
       <c r="F23" s="147">
         <v>45600</v>
       </c>
@@ -12770,9 +12696,7 @@
       <c r="F27" s="149">
         <v>454856</v>
       </c>
-      <c r="G27" s="149">
-        <v>1051437</v>
-      </c>
+      <c r="G27" s="149"/>
       <c r="H27" s="149">
         <v>854800</v>
       </c>
@@ -13176,7 +13100,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" zeroHeight="1"/>
@@ -13380,9 +13304,7 @@
       <c r="E14" s="147">
         <v>143845</v>
       </c>
-      <c r="F14" s="147">
-        <v>17183</v>
-      </c>
+      <c r="F14" s="147"/>
       <c r="G14" s="147">
         <v>690766</v>
       </c>
@@ -13420,9 +13342,7 @@
       <c r="C16" s="147">
         <v>58790</v>
       </c>
-      <c r="D16" s="147">
-        <v>888542</v>
-      </c>
+      <c r="D16" s="147"/>
       <c r="E16" s="147">
         <v>224222</v>
       </c>
@@ -13531,9 +13451,7 @@
       <c r="F20" s="147">
         <v>127211</v>
       </c>
-      <c r="G20" s="147">
-        <v>2114554</v>
-      </c>
+      <c r="G20" s="147"/>
       <c r="K20" s="91"/>
       <c r="L20" s="91"/>
       <c r="M20" s="91"/>
@@ -13603,9 +13521,7 @@
       <c r="B23" s="147">
         <v>12585169</v>
       </c>
-      <c r="C23" s="147">
-        <v>689647</v>
-      </c>
+      <c r="C23" s="147"/>
       <c r="D23" s="147">
         <v>13274816</v>
       </c>
@@ -14206,8 +14122,8 @@
   <dimension ref="A1:BF266"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="11" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" activeCellId="7" sqref="G40 K34 N18 P28 P39 Q54 L57 E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" zeroHeight="1"/>
@@ -14813,9 +14729,7 @@
       <c r="M18" s="147">
         <v>22673</v>
       </c>
-      <c r="N18" s="147">
-        <v>40306</v>
-      </c>
+      <c r="N18" s="147"/>
       <c r="O18" s="147">
         <v>9982</v>
       </c>
@@ -15318,7 +15232,7 @@
         <v>267465</v>
       </c>
       <c r="D28" s="149">
-        <v>416491</v>
+        <v>416481</v>
       </c>
       <c r="E28" s="149">
         <v>699302</v>
@@ -15353,9 +15267,7 @@
       <c r="O28" s="149">
         <v>255125</v>
       </c>
-      <c r="P28" s="149">
-        <v>480789</v>
-      </c>
+      <c r="P28" s="149"/>
       <c r="Q28" s="149">
         <v>774155</v>
       </c>
@@ -15614,9 +15526,7 @@
       <c r="J34" s="147">
         <v>23566</v>
       </c>
-      <c r="K34" s="147">
-        <v>15997</v>
-      </c>
+      <c r="K34" s="147"/>
       <c r="L34" s="147">
         <v>14106</v>
       </c>
@@ -15914,9 +15824,7 @@
       <c r="O39" s="147">
         <v>755</v>
       </c>
-      <c r="P39" s="147">
-        <v>1736</v>
-      </c>
+      <c r="P39" s="147"/>
       <c r="Q39" s="147">
         <v>9714</v>
       </c>
@@ -15944,9 +15852,7 @@
       <c r="F40" s="147">
         <v>167118</v>
       </c>
-      <c r="G40" s="147">
-        <v>143715</v>
-      </c>
+      <c r="G40" s="147"/>
       <c r="H40" s="147">
         <v>110850</v>
       </c>
@@ -16577,9 +16483,7 @@
       <c r="D53" s="147">
         <v>9892</v>
       </c>
-      <c r="E53" s="147">
-        <v>30460</v>
-      </c>
+      <c r="E53" s="147"/>
       <c r="F53" s="147">
         <v>49310</v>
       </c>
@@ -16670,9 +16574,7 @@
       <c r="P54" s="147">
         <v>22676</v>
       </c>
-      <c r="Q54" s="147">
-        <v>37481</v>
-      </c>
+      <c r="Q54" s="147"/>
       <c r="R54" s="147">
         <v>1191393</v>
       </c>
@@ -16826,9 +16728,7 @@
       <c r="K57" s="147">
         <v>12609</v>
       </c>
-      <c r="L57" s="147">
-        <v>10268</v>
-      </c>
+      <c r="L57" s="147"/>
       <c r="M57" s="147">
         <v>6218</v>
       </c>
@@ -17716,8 +17616,8 @@
   <dimension ref="A1:Q193"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="12" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.25" zeroHeight="1"/>
@@ -17901,17 +17801,13 @@
       <c r="D15" s="147">
         <v>8337</v>
       </c>
-      <c r="E15" s="147">
-        <v>790053</v>
-      </c>
+      <c r="E15" s="147"/>
     </row>
     <row r="16" spans="1:17" ht="11.1" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="147">
-        <v>80262</v>
-      </c>
+      <c r="B16" s="147"/>
       <c r="C16" s="147">
         <v>822180</v>
       </c>
@@ -17983,9 +17879,7 @@
       <c r="C20" s="147">
         <v>468132</v>
       </c>
-      <c r="D20" s="147">
-        <v>6603</v>
-      </c>
+      <c r="D20" s="147"/>
       <c r="E20" s="147">
         <v>605094</v>
       </c>
@@ -18048,9 +17942,7 @@
       <c r="B24" s="147">
         <v>54758</v>
       </c>
-      <c r="C24" s="147">
-        <v>70711</v>
-      </c>
+      <c r="C24" s="147"/>
       <c r="D24" s="147">
         <v>1819</v>
       </c>
@@ -18216,9 +18108,7 @@
       <c r="B35" s="147">
         <v>78681</v>
       </c>
-      <c r="C35" s="147">
-        <v>299688</v>
-      </c>
+      <c r="C35" s="147"/>
       <c r="D35" s="147">
         <v>3853</v>
       </c>
@@ -18239,9 +18129,7 @@
       <c r="D36" s="147">
         <v>4352</v>
       </c>
-      <c r="E36" s="147">
-        <v>111003</v>
-      </c>
+      <c r="E36" s="147"/>
     </row>
     <row r="37" spans="1:17" ht="11.1" customHeight="1">
       <c r="A37" s="18" t="s">
@@ -18264,9 +18152,7 @@
       <c r="A38" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="147">
-        <v>130979</v>
-      </c>
+      <c r="B38" s="147"/>
       <c r="C38" s="147">
         <v>257453</v>
       </c>
@@ -18321,9 +18207,7 @@
       <c r="C41" s="147">
         <v>1114471</v>
       </c>
-      <c r="D41" s="147">
-        <v>11410</v>
-      </c>
+      <c r="D41" s="147"/>
       <c r="E41" s="147">
         <v>1359011</v>
       </c>
@@ -18700,9 +18584,7 @@
       <c r="C65" s="149">
         <v>22464703</v>
       </c>
-      <c r="D65" s="149">
-        <v>1493676</v>
-      </c>
+      <c r="D65" s="149"/>
       <c r="E65" s="149">
         <v>25422788</v>
       </c>
@@ -19023,9 +18905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915BBABF-51E6-4CBA-AC78-98E696CFC099}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" activeCellId="9" sqref="B14 E24 F20 G15 G37 F40 E35 C33 B46 D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" zeroHeight="1"/>
@@ -19194,9 +19076,7 @@
       <c r="A14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="164">
-        <v>267086</v>
-      </c>
+      <c r="B14" s="164"/>
       <c r="C14" s="164">
         <v>14760</v>
       </c>
@@ -19232,9 +19112,7 @@
       <c r="F15" s="164">
         <v>5015</v>
       </c>
-      <c r="G15" s="164">
-        <v>733991</v>
-      </c>
+      <c r="G15" s="164"/>
     </row>
     <row r="16" spans="1:7" ht="11.1" customHeight="1">
       <c r="A16" s="18" t="s">
@@ -19344,9 +19222,7 @@
       <c r="E20" s="164">
         <v>83408</v>
       </c>
-      <c r="F20" s="164">
-        <v>2328</v>
-      </c>
+      <c r="F20" s="164"/>
       <c r="G20" s="164">
         <v>116458</v>
       </c>
@@ -19433,9 +19309,7 @@
       <c r="D24" s="164">
         <v>371031</v>
       </c>
-      <c r="E24" s="164">
-        <v>398624</v>
-      </c>
+      <c r="E24" s="164"/>
       <c r="F24" s="164">
         <v>8344</v>
       </c>
@@ -19580,9 +19454,7 @@
       <c r="B33" s="164">
         <v>569418</v>
       </c>
-      <c r="C33" s="164">
-        <v>31154</v>
-      </c>
+      <c r="C33" s="164"/>
       <c r="D33" s="164">
         <v>600571</v>
       </c>
@@ -19632,9 +19504,7 @@
       <c r="D35" s="164">
         <v>1626</v>
       </c>
-      <c r="E35" s="164">
-        <v>99476</v>
-      </c>
+      <c r="E35" s="164"/>
       <c r="F35" s="164">
         <v>9774</v>
       </c>
@@ -19684,9 +19554,7 @@
       <c r="F37" s="164">
         <v>10236</v>
       </c>
-      <c r="G37" s="164">
-        <v>390417</v>
-      </c>
+      <c r="G37" s="164"/>
     </row>
     <row r="38" spans="1:7" ht="11.1" customHeight="1">
       <c r="A38" s="18" t="s">
@@ -19750,9 +19618,7 @@
       <c r="E40" s="164">
         <v>562415</v>
       </c>
-      <c r="F40" s="164">
-        <v>13161</v>
-      </c>
+      <c r="F40" s="164"/>
       <c r="G40" s="164">
         <v>1313254</v>
       </c>
@@ -19862,9 +19728,7 @@
       <c r="A46" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="165">
-        <v>5849207</v>
-      </c>
+      <c r="B46" s="165"/>
       <c r="C46" s="165">
         <v>295199</v>
       </c>
@@ -20012,9 +19876,7 @@
       <c r="C54" s="164">
         <v>25010</v>
       </c>
-      <c r="D54" s="164">
-        <v>421642</v>
-      </c>
+      <c r="D54" s="164"/>
       <c r="E54" s="164">
         <v>751498</v>
       </c>

</xml_diff>